<commit_message>
Updated progress for calendar min price
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
   <si>
     <t xml:space="preserve">Métricas</t>
   </si>
@@ -49,13 +49,19 @@
     <t xml:space="preserve">Finished</t>
   </si>
   <si>
-    <t xml:space="preserve">Listing con mayor precio promedio</t>
+    <t xml:space="preserve">Listing disponible con mayor precio promedio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calendar_max_money.py</t>
   </si>
   <si>
     <t xml:space="preserve">Por País</t>
   </si>
   <si>
-    <t xml:space="preserve">Listing con menor precio promedio</t>
+    <t xml:space="preserve">Listing disponible con menor precio promedio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calendar_min_money.py</t>
   </si>
   <si>
     <t xml:space="preserve">Listing con mayor número de reviews</t>
@@ -101,9 +107,6 @@
   </si>
   <si>
     <t xml:space="preserve">Listing que generó más ingresos para su host</t>
-  </si>
-  <si>
-    <t xml:space="preserve">calendar_max_money.py</t>
   </si>
   <si>
     <t xml:space="preserve">Porcentaje de arriendos en fechas festivas</t>
@@ -137,7 +140,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -170,15 +173,27 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3399FF"/>
+        <bgColor rgb="FF33CCCC"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -200,12 +215,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF3399FF"/>
-        <bgColor rgb="FF33CCCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
         <bgColor rgb="FFCCFFCC"/>
       </patternFill>
@@ -214,6 +223,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00CC00"/>
         <bgColor rgb="FF00CC33"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66CCFF"/>
+        <bgColor rgb="FF33CCCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -233,7 +248,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -257,17 +272,20 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -275,14 +293,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -291,22 +309,31 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Untitled1" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
@@ -329,7 +356,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FF0066FF"/>
+          <bgColor rgb="FF3399FF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -370,7 +397,7 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066FF"/>
+      <rgbColor rgb="FF0066CC"/>
       <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
@@ -384,7 +411,7 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FF66CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
@@ -417,20 +444,20 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F31" activeCellId="0" sqref="F31"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.6428571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.26020408163265"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.3979591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.65816326530612"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.3265306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.9948979591837"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -504,269 +531,271 @@
         <v>9</v>
       </c>
       <c r="B7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" s="9"/>
+        <v>2</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="D7" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C8" s="9"/>
+        <v>12</v>
+      </c>
+      <c r="B8" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>13</v>
+      </c>
       <c r="D8" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="8" t="n">
+        <v>14</v>
+      </c>
+      <c r="B9" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>13</v>
+      <c r="C9" s="11" t="s">
+        <v>15</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" s="9"/>
+        <v>16</v>
+      </c>
+      <c r="B10" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="11"/>
       <c r="D10" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" s="9"/>
+        <v>17</v>
+      </c>
+      <c r="B11" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="11"/>
       <c r="D11" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" s="9"/>
+        <v>18</v>
+      </c>
+      <c r="B12" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" s="11"/>
       <c r="D12" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C13" s="9"/>
+        <v>19</v>
+      </c>
+      <c r="B13" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="11"/>
       <c r="D13" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C14" s="9"/>
+        <v>20</v>
+      </c>
+      <c r="B14" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="11"/>
       <c r="D14" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C15" s="9"/>
+        <v>21</v>
+      </c>
+      <c r="B15" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" s="11"/>
       <c r="D15" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="8" t="n">
+        <v>22</v>
+      </c>
+      <c r="B16" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>21</v>
+      <c r="C16" s="11" t="s">
+        <v>23</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C17" s="9"/>
+        <v>24</v>
+      </c>
+      <c r="B17" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" s="11"/>
       <c r="D17" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C18" s="9"/>
+        <v>25</v>
+      </c>
+      <c r="B18" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" s="11"/>
       <c r="D18" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C19" s="9"/>
+        <v>26</v>
+      </c>
+      <c r="B19" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" s="11"/>
       <c r="D19" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C20" s="9"/>
+        <v>27</v>
+      </c>
+      <c r="B20" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" s="11"/>
       <c r="D20" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>27</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="B21" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" s="11"/>
       <c r="D21" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C22" s="9"/>
+        <v>29</v>
+      </c>
+      <c r="B22" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" s="11"/>
       <c r="D22" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B23" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C23" s="9"/>
+        <v>30</v>
+      </c>
+      <c r="B23" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" s="11"/>
       <c r="D23" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C24" s="9"/>
+        <v>31</v>
+      </c>
+      <c r="B24" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" s="11"/>
       <c r="D24" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C25" s="9"/>
+        <v>32</v>
+      </c>
+      <c r="B25" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" s="11"/>
       <c r="D25" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C26" s="9"/>
+        <v>33</v>
+      </c>
+      <c r="B26" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" s="11"/>
       <c r="D26" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C27" s="11"/>
+      <c r="D27" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="B27" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B28" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C28" s="9"/>
+        <v>36</v>
+      </c>
+      <c r="B28" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C28" s="11"/>
       <c r="D28" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified shrek for output name
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
   <si>
     <t xml:space="preserve">Métricas</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t xml:space="preserve">Listing que se ha arrendado más veces</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMPLETADO</t>
   </si>
   <si>
     <t xml:space="preserve">Listings disponibles entre un rango de fechas</t>
@@ -137,8 +140,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.00%"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -173,13 +177,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -188,12 +192,6 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF3399FF"/>
-        <bgColor rgb="FF33CCCC"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -211,6 +209,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF3300"/>
         <bgColor rgb="FFFF6600"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3399FF"/>
+        <bgColor rgb="FF33CCCC"/>
       </patternFill>
     </fill>
     <fill>
@@ -248,7 +252,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -272,20 +276,17 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -293,14 +294,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -321,19 +322,26 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Untitled1" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
@@ -441,23 +449,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.9948979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.6428571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.26020408163265"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.8775510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.65816326530612"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.7704081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -547,7 +552,7 @@
       <c r="B8" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -561,7 +566,7 @@
       <c r="B9" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="9" t="s">
         <v>15</v>
       </c>
       <c r="D9" s="3" t="s">
@@ -575,80 +580,105 @@
       <c r="B10" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="C10" s="11"/>
+      <c r="C10" s="9"/>
       <c r="D10" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="F10" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B11" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="C11" s="11"/>
+      <c r="C11" s="9"/>
       <c r="D11" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B12" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="C12" s="11"/>
+      <c r="C12" s="9"/>
       <c r="D12" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="F12" s="12" t="n">
+        <f aca="false">SUMIF(B7:B28,"=2")/2/COUNT(B7:B28)</f>
+        <v>0.227272727272727</v>
+      </c>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B13" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="C13" s="11"/>
+      <c r="C13" s="9"/>
       <c r="D13" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B14" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="C14" s="11"/>
+      <c r="C14" s="9"/>
       <c r="D14" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B15" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="C15" s="11"/>
+      <c r="C15" s="9"/>
       <c r="D15" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B16" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="C16" s="11" t="s">
-        <v>23</v>
+      <c r="C16" s="9" t="s">
+        <v>24</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>11</v>
@@ -656,152 +686,156 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B17" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="C17" s="11"/>
+      <c r="C17" s="9"/>
       <c r="D17" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B18" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="C18" s="11"/>
+      <c r="C18" s="9"/>
       <c r="D18" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B19" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="C19" s="11"/>
+      <c r="C19" s="9"/>
       <c r="D19" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B20" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="C20" s="11"/>
+      <c r="C20" s="9"/>
       <c r="D20" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B21" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="C21" s="11"/>
+      <c r="C21" s="9"/>
       <c r="D21" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B22" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="C22" s="11"/>
+      <c r="C22" s="9"/>
       <c r="D22" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B23" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="C23" s="11"/>
+      <c r="C23" s="9"/>
       <c r="D23" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B24" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="C24" s="11"/>
+      <c r="C24" s="9"/>
       <c r="D24" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B25" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="C25" s="11"/>
+      <c r="C25" s="9"/>
       <c r="D25" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B26" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C26" s="11"/>
+        <v>2</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>24</v>
+      </c>
       <c r="D26" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C27" s="9"/>
+      <c r="D27" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="B27" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C27" s="11"/>
-      <c r="D27" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B28" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="C28" s="11"/>
+      <c r="C28" s="9"/>
       <c r="D28" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:D4"/>
     <mergeCell ref="F2:G3"/>
+    <mergeCell ref="F10:I11"/>
+    <mergeCell ref="F12:I14"/>
   </mergeCells>
   <conditionalFormatting sqref="B7:B28">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">

</xml_diff>

<commit_message>
Implemented 4 new metrics and modified previous ones
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="48">
   <si>
     <t xml:space="preserve">Métricas</t>
   </si>
@@ -70,7 +70,13 @@
     <t xml:space="preserve">reviews_max_reviews_by_listing.py</t>
   </si>
   <si>
-    <t xml:space="preserve">Listing que se ha arrendado más veces</t>
+    <t xml:space="preserve">Listing con más reservas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calendar_most_rented.py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*</t>
   </si>
   <si>
     <t xml:space="preserve">COMPLETADO</t>
@@ -79,9 +85,21 @@
     <t xml:space="preserve">Listings disponibles entre un rango de fechas</t>
   </si>
   <si>
+    <t xml:space="preserve">calendar_available_between_dates.py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**</t>
+  </si>
+  <si>
     <t xml:space="preserve">Listing más barato disponible entre un rango de fechas</t>
   </si>
   <si>
+    <t xml:space="preserve">calendar_cheapest_available_between_dates.py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">***</t>
+  </si>
+  <si>
     <t xml:space="preserve">Listing con mejor rating entre los listings más baratos</t>
   </si>
   <si>
@@ -100,10 +118,22 @@
     <t xml:space="preserve">Usuario con mayor número de reviews</t>
   </si>
   <si>
+    <t xml:space="preserve">reviews_max_reviews_by_user.py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“listing que se ha arrendado más veces” no puede ser ya que calendar son los listings “futuros” a partir de mayo 2017</t>
+  </si>
+  <si>
     <t xml:space="preserve">Usuario más disconforme en sus reviews</t>
   </si>
   <si>
+    <t xml:space="preserve">Se entregan los listings que estan disponibles en TODO el intervalo</t>
+  </si>
+  <si>
     <t xml:space="preserve">Usuarios que se arrienden listings mutuamente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entrega el listing con el precio TOTAL mínimo entre los listings disponibles durante TODO el intervalo</t>
   </si>
   <si>
     <t xml:space="preserve">Par de usuarios con mayor similitud en listings visitados</t>
@@ -144,7 +174,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -178,12 +208,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -277,7 +301,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -328,10 +352,6 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -457,12 +477,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.6428571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.26020408163265"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.8775510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.65816326530612"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.3367346938776"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -578,14 +600,19 @@
         <v>16</v>
       </c>
       <c r="B10" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" s="9"/>
+        <v>2</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>17</v>
+      </c>
       <c r="D10" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="E10" s="0" t="s">
+        <v>18</v>
+      </c>
       <c r="F10" s="11" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
@@ -593,14 +620,19 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B11" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" s="9"/>
+        <v>2</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>21</v>
+      </c>
       <c r="D11" s="3" t="s">
         <v>11</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>22</v>
       </c>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
@@ -609,18 +641,23 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B12" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" s="9"/>
+        <v>2</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>24</v>
+      </c>
       <c r="D12" s="3" t="s">
         <v>11</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="F12" s="12" t="n">
         <f aca="false">SUMIF(B7:B28,"=2")/2/COUNT(B7:B28)</f>
-        <v>0.227272727272727</v>
+        <v>0.363636363636364</v>
       </c>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
@@ -628,7 +665,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B13" s="10" t="n">
         <v>0</v>
@@ -644,7 +681,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B14" s="10" t="n">
         <v>0</v>
@@ -660,7 +697,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B15" s="10" t="n">
         <v>0</v>
@@ -672,13 +709,13 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B16" s="10" t="n">
         <v>2</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>11</v>
@@ -686,19 +723,27 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B17" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C17" s="9"/>
+        <v>2</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="D17" s="3" t="s">
         <v>11</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B18" s="10" t="n">
         <v>0</v>
@@ -707,10 +752,16 @@
       <c r="D18" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="F18" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B19" s="10" t="n">
         <v>0</v>
@@ -719,10 +770,16 @@
       <c r="D19" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="F19" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B20" s="10" t="n">
         <v>0</v>
@@ -734,7 +791,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="B21" s="10" t="n">
         <v>0</v>
@@ -746,7 +803,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B22" s="10" t="n">
         <v>0</v>
@@ -758,7 +815,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="B23" s="10" t="n">
         <v>0</v>
@@ -770,7 +827,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="B24" s="10" t="n">
         <v>0</v>
@@ -782,7 +839,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="B25" s="10" t="n">
         <v>0</v>
@@ -794,40 +851,38 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B26" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>24</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C26" s="9"/>
       <c r="D26" s="3" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="B27" s="10" t="n">
         <v>0</v>
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="3" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="B28" s="10" t="n">
         <v>0</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="3" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
agregada nueva metrica al excel
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
   <si>
     <t>Métricas</t>
   </si>
@@ -156,6 +156,9 @@
   </si>
   <si>
     <t>General</t>
+  </si>
+  <si>
+    <t>Promedio arriendo mes, semana, año.</t>
   </si>
   <si>
     <t>Usuario con reviews en más países</t>
@@ -248,7 +251,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00CC00"/>
-        <bgColor rgb="FF00CC33"/>
+        <bgColor rgb="FF008000"/>
       </patternFill>
     </fill>
     <fill>
@@ -361,6 +364,17 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </dxf>
+  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -412,7 +426,7 @@
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF00CC33"/>
+      <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
@@ -429,10 +443,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C39" activeCellId="0" sqref="C39"/>
+      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -832,7 +846,7 @@
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="3" t="s">
-        <v>46</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -844,6 +858,18 @@
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C29" s="9"/>
+      <c r="D29" s="3" t="s">
         <v>46</v>
       </c>
     </row>
@@ -854,7 +880,7 @@
     <mergeCell ref="F10:I11"/>
     <mergeCell ref="F12:I14"/>
   </mergeCells>
-  <conditionalFormatting sqref="B7:B28">
+  <conditionalFormatting sqref="B7:B29">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
add number of rooms to excel
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -5,220 +5,221 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="474" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="66">
-  <si>
-    <t xml:space="preserve">Métricas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leyenda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not Implemented</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In Progress</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nombre Archivo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tipo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Finished</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Listing disponible con mayor precio promedio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">calendar_max_money.py</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Por País</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Listing disponible con menor precio promedio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">calendar_min_money.py</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Listing con mayor número de reviews</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reviews_max_reviews_by_listing.py</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Listing con más reservas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">calendar_most_rented.py</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMPLETADO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Listings disponibles entre un rango de fechas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">calendar_available_between_dates.py</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Listing más barato disponible entre un rango de fechas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">calendar_cheapest_available_between_dates.py</t>
-  </si>
-  <si>
-    <t xml:space="preserve">***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Listing con mejor rating entre los listings más baratos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Listing más barato entre los listings con mejor rating</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Listing con reviews más negativos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Usuario con más listings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">listing_max_number_of_user_listing.py</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Usuario con mayor número de reviews</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reviews_max_reviews_by_user.py</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“listing que se ha arrendado más veces” no puede ser ya que calendar son los listings “futuros” a partir de mayo 2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Usuario más disconforme en sus reviews</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Se entregan los listings que estan disponibles en TODO el intervalo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Usuarios que se arrienden listings mutuamente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entrega el listing con el precio TOTAL mínimo entre los listings disponibles durante TODO el intervalo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Par de usuarios con mayor similitud en listings visitados</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Listing que generó más ingresos para su host en un año</t>
-  </si>
-  <si>
-    <t xml:space="preserve">listing_max_value_generate.py</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Porcentaje de arriendos en fechas festivas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Promedio del valor de cada cama</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Promedio del número de baños en relación a los huespedes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Número de listings por barrio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Usuario con listings en más países</t>
-  </si>
-  <si>
-    <t xml:space="preserve">General</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Promedio arriendo mes, semana, año.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Usuario con reviews en más países</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comparativa de precio promedio entre países</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amsterdam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dublin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HongKong</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NewYork</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paris</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n° of Bedrooms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Property Buying Price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Avg Listing price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Avg Reviews (rents) per listing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Avg rents per Year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Avg Income per Year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 bedroom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 bedrooms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 bedrooms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 bedrooms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5+ bedrooms</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="68">
+  <si>
+    <t>Métricas</t>
+  </si>
+  <si>
+    <t>Leyenda</t>
+  </si>
+  <si>
+    <t>Not Implemented</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Descripción</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>Nombre Archivo</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Finished</t>
+  </si>
+  <si>
+    <t>Listing disponible con mayor precio promedio</t>
+  </si>
+  <si>
+    <t>calendar_max_money.py</t>
+  </si>
+  <si>
+    <t>Por País</t>
+  </si>
+  <si>
+    <t>Listing disponible con menor precio promedio</t>
+  </si>
+  <si>
+    <t>calendar_min_money.py</t>
+  </si>
+  <si>
+    <t>Listing con mayor número de reviews</t>
+  </si>
+  <si>
+    <t>reviews_max_reviews_by_listing.py</t>
+  </si>
+  <si>
+    <t>Listing con más reservas</t>
+  </si>
+  <si>
+    <t>calendar_most_rented.py</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>COMPLETADO</t>
+  </si>
+  <si>
+    <t>Listings disponibles entre un rango de fechas</t>
+  </si>
+  <si>
+    <t>calendar_available_between_dates.py</t>
+  </si>
+  <si>
+    <t>**</t>
+  </si>
+  <si>
+    <t>Listing más barato disponible entre un rango de fechas</t>
+  </si>
+  <si>
+    <t>calendar_cheapest_available_between_dates.py</t>
+  </si>
+  <si>
+    <t>***</t>
+  </si>
+  <si>
+    <t>Listing con mejor rating entre los listings más baratos</t>
+  </si>
+  <si>
+    <t>Listing más barato entre los listings con mejor rating</t>
+  </si>
+  <si>
+    <t>Listing con reviews más negativos</t>
+  </si>
+  <si>
+    <t>Usuario con más listings</t>
+  </si>
+  <si>
+    <t>listing_max_number_of_user_listing.py</t>
+  </si>
+  <si>
+    <t>Usuario con mayor número de reviews</t>
+  </si>
+  <si>
+    <t>reviews_max_reviews_by_user.py</t>
+  </si>
+  <si>
+    <t>“listing que se ha arrendado más veces” no puede ser ya que calendar son los listings “futuros” a partir de mayo 2017</t>
+  </si>
+  <si>
+    <t>Usuario más disconforme en sus reviews</t>
+  </si>
+  <si>
+    <t>Se entregan los listings que estan disponibles en TODO el intervalo</t>
+  </si>
+  <si>
+    <t>Usuarios que se arrienden listings mutuamente</t>
+  </si>
+  <si>
+    <t>Entrega el listing con el precio TOTAL mínimo entre los listings disponibles durante TODO el intervalo</t>
+  </si>
+  <si>
+    <t>Par de usuarios con mayor similitud en listings visitados</t>
+  </si>
+  <si>
+    <t>Listing que generó más ingresos para su host en un año</t>
+  </si>
+  <si>
+    <t>listing_max_value_generate.py</t>
+  </si>
+  <si>
+    <t>Porcentaje de arriendos en fechas festivas</t>
+  </si>
+  <si>
+    <t>Promedio del valor de cada cama</t>
+  </si>
+  <si>
+    <t>Promedio del número de baños en relación a los huespedes</t>
+  </si>
+  <si>
+    <t>Número de listings por barrio</t>
+  </si>
+  <si>
+    <t>Usuario con listings en más países</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Promedio arriendo mes, semana, año.</t>
+  </si>
+  <si>
+    <t>Usuario con reviews en más países</t>
+  </si>
+  <si>
+    <t>Comparativa de precio promedio entre países</t>
+  </si>
+  <si>
+    <t>Amsterdam</t>
+  </si>
+  <si>
+    <t>Dublin</t>
+  </si>
+  <si>
+    <t>HongKong</t>
+  </si>
+  <si>
+    <t>NewYork</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>n° of Bedrooms</t>
+  </si>
+  <si>
+    <t>Property Buying Price</t>
+  </si>
+  <si>
+    <t>Avg Listing price</t>
+  </si>
+  <si>
+    <t>Avg Reviews (rents) per listing</t>
+  </si>
+  <si>
+    <t>Avg rents per Year</t>
+  </si>
+  <si>
+    <t>Avg Income per Year</t>
+  </si>
+  <si>
+    <t>AVG</t>
+  </si>
+  <si>
+    <t>1 bedroom</t>
+  </si>
+  <si>
+    <t>2 bedrooms</t>
+  </si>
+  <si>
+    <t>3 bedrooms</t>
+  </si>
+  <si>
+    <t>4 bedrooms</t>
+  </si>
+  <si>
+    <t>5+ bedrooms</t>
+  </si>
+  <si>
+    <t>Error ( 0 )</t>
   </si>
 </sst>
 </file>
@@ -226,7 +227,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0.00%"/>
   </numFmts>
   <fonts count="6">
@@ -425,9 +426,10 @@
   <dxfs count="3">
     <dxf>
       <font>
+        <sz val="10"/>
         <name val="Arial"/>
+        <family val="2"/>
         <charset val="1"/>
-        <family val="2"/>
       </font>
       <fill>
         <patternFill>
@@ -437,9 +439,10 @@
     </dxf>
     <dxf>
       <font>
+        <sz val="10"/>
         <name val="Arial"/>
+        <family val="2"/>
         <charset val="1"/>
-        <family val="2"/>
       </font>
       <fill>
         <patternFill>
@@ -449,9 +452,10 @@
     </dxf>
     <dxf>
       <font>
+        <sz val="10"/>
         <name val="Arial"/>
+        <family val="2"/>
         <charset val="1"/>
-        <family val="2"/>
       </font>
       <fill>
         <patternFill>
@@ -539,8 +543,11 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.1122448979592"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.75"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.3367346938776"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.72959183673469"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="8.72959183673469"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -977,8 +984,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -988,10 +995,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1065,30 +1072,156 @@
       <c r="F11" s="0" t="s">
         <v>54</v>
       </c>
+      <c r="G11" s="0" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>9266</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>4636</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>4523</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>32320</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>33597</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <f aca="false">(B12+C12+D12+E12+F12)/5</f>
+        <v>16868.4</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>3487</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>1329</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>934</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>5570</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>8242</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <f aca="false">(B13+C13+D13+E13+F13)/5</f>
+        <v>3912.4</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>402</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>382</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>1707</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>2185</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <f aca="false">(B14+C14+D14+E14+F14)/5</f>
+        <v>936.8</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>362</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>180</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>457</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>511</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <f aca="false">(B15+C15+D15+E15+F15)/5</f>
+        <v>313.4</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <f aca="false">10+18+7+3+2</f>
+        <v>40</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <f aca="false">14+4+4+1</f>
+        <v>23</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <f aca="false">104+26+4+11+5+2</f>
+        <v>152</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <f aca="false">3+6+4+23+95+1</f>
+        <v>132</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <f aca="false">(B16+C16+D16+E16+F16)/5</f>
+        <v>79.2</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>901</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>131</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>548</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>4037</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>11740</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <f aca="false">(B17+C17+D17+E17+F17)/5</f>
+        <v>3471.4</v>
       </c>
     </row>
   </sheetData>
@@ -1096,8 +1229,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>